<commit_message>
guys, u r killing me with this
</commit_message>
<xml_diff>
--- a/Data by Year:Prov:TOTALS/Data by Year_Prov_TOTALS/ALL_DATA_PROV.xlsx
+++ b/Data by Year:Prov:TOTALS/Data by Year_Prov_TOTALS/ALL_DATA_PROV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyaczeban/Desktop/Data by Year:Prov/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyaczeban/Desktop/class/group10_project/Data by Year:Prov:TOTALS/Data by Year_Prov_TOTALS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D806FCC-1C24-864B-A7C4-CB85EEF258E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A18318FE-0E2B-2640-9199-3A565DED7CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5200" yWindow="500" windowWidth="18620" windowHeight="15600" xr2:uid="{7B27A209-A6C5-D043-BF0C-084A329AC59C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Kilotonnes</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Population</t>
-  </si>
-  <si>
-    <t>Canada/Totals</t>
   </si>
 </sst>
 </file>
@@ -453,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570C482B-B5CC-3346-9046-0FEEA3259D2F}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A2" sqref="A2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,149 +495,164 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2015</v>
       </c>
+      <c r="C2">
+        <v>299300</v>
+      </c>
       <c r="D2" s="1">
-        <v>766744</v>
+        <v>11299</v>
       </c>
       <c r="E2">
-        <v>69970.600000000006</v>
-      </c>
-      <c r="F2" s="1">
-        <v>206105</v>
+        <v>6370.75</v>
+      </c>
+      <c r="F2">
+        <v>390</v>
       </c>
       <c r="G2" s="1">
-        <v>31200</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3406089</v>
+        <v>35200</v>
+      </c>
+      <c r="H2">
+        <v>341412</v>
       </c>
       <c r="I2" s="1">
-        <v>142712260</v>
+        <v>2113237</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2016</v>
       </c>
+      <c r="C3">
+        <v>298800</v>
+      </c>
       <c r="D3" s="1">
-        <v>741903</v>
+        <v>11636</v>
       </c>
       <c r="E3">
-        <v>71236.009999999995</v>
-      </c>
-      <c r="F3" s="1">
-        <v>207080</v>
+        <v>6500.63</v>
+      </c>
+      <c r="F3">
+        <v>345</v>
       </c>
       <c r="G3" s="1">
-        <v>32100</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3405282</v>
+        <v>40700</v>
+      </c>
+      <c r="H3">
+        <v>342472</v>
       </c>
       <c r="I3" s="1">
-        <v>144209652</v>
+        <v>2117189</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2017</v>
       </c>
+      <c r="C4">
+        <v>294900</v>
+      </c>
       <c r="D4" s="1">
-        <v>756590</v>
+        <v>11505</v>
       </c>
       <c r="E4">
-        <v>70996.289999999994</v>
-      </c>
-      <c r="F4" s="1">
-        <v>207825</v>
+        <v>6042.04</v>
+      </c>
+      <c r="F4">
+        <v>285</v>
       </c>
       <c r="G4" s="1">
-        <v>33700</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3479555</v>
+        <v>45600</v>
+      </c>
+      <c r="H4">
+        <v>343966</v>
       </c>
       <c r="I4" s="1">
-        <v>145978571</v>
+        <v>2114428</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2018</v>
       </c>
+      <c r="C5">
+        <v>285000</v>
+      </c>
       <c r="D5" s="1">
-        <v>771446</v>
+        <v>11337</v>
       </c>
       <c r="E5">
-        <v>72155.62</v>
-      </c>
-      <c r="F5" s="1">
-        <v>210185</v>
+        <v>6041.56</v>
+      </c>
+      <c r="F5">
+        <v>300</v>
       </c>
       <c r="G5" s="1">
-        <v>35700</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3525571</v>
+        <v>45100</v>
+      </c>
+      <c r="H5">
+        <v>346836</v>
       </c>
       <c r="I5" s="1">
-        <v>148012308</v>
+        <v>2105228</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>2019</v>
       </c>
+      <c r="C6">
+        <v>272700</v>
+      </c>
       <c r="D6" s="1">
-        <v>771813</v>
+        <v>11277</v>
       </c>
       <c r="E6">
-        <v>77563.350000000006</v>
-      </c>
-      <c r="F6" s="1">
-        <v>212485</v>
+        <v>6686.65</v>
+      </c>
+      <c r="F6">
+        <v>300</v>
       </c>
       <c r="G6" s="1">
-        <v>36900</v>
-      </c>
-      <c r="H6" s="1">
-        <v>3609093</v>
+        <v>47100</v>
+      </c>
+      <c r="H6">
+        <v>349654</v>
       </c>
       <c r="I6" s="1">
-        <v>150160810</v>
+        <v>2096208</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>2015</v>
       </c>
       <c r="C7">
-        <v>299300</v>
+        <v>204200</v>
       </c>
       <c r="D7" s="1">
-        <v>11299</v>
+        <v>1584</v>
       </c>
       <c r="E7">
-        <v>6370.75</v>
+        <v>4750.04</v>
       </c>
       <c r="F7">
-        <v>390</v>
+        <v>325</v>
       </c>
       <c r="G7" s="1">
-        <v>35200</v>
+        <v>17500</v>
       </c>
       <c r="H7">
-        <v>341412</v>
+        <v>292544</v>
       </c>
       <c r="I7" s="1">
-        <v>2113237</v>
+        <v>578067</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -648,25 +660,25 @@
         <v>2016</v>
       </c>
       <c r="C8">
-        <v>298800</v>
+        <v>214700</v>
       </c>
       <c r="D8" s="1">
-        <v>11636</v>
+        <v>1712</v>
       </c>
       <c r="E8">
-        <v>6500.63</v>
+        <v>5012.62</v>
       </c>
       <c r="F8">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="G8" s="1">
-        <v>40700</v>
+        <v>23200</v>
       </c>
       <c r="H8">
-        <v>342472</v>
+        <v>292419</v>
       </c>
       <c r="I8" s="1">
-        <v>2117189</v>
+        <v>585891</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -674,25 +686,25 @@
         <v>2017</v>
       </c>
       <c r="C9">
-        <v>294900</v>
+        <v>240400</v>
       </c>
       <c r="D9" s="1">
-        <v>11505</v>
+        <v>1762</v>
       </c>
       <c r="E9">
-        <v>6042.04</v>
+        <v>4713.37</v>
       </c>
       <c r="F9">
-        <v>285</v>
+        <v>325</v>
       </c>
       <c r="G9" s="1">
-        <v>45600</v>
+        <v>22300</v>
       </c>
       <c r="H9">
-        <v>343966</v>
+        <v>299369</v>
       </c>
       <c r="I9" s="1">
-        <v>2114428</v>
+        <v>598819</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -700,25 +712,25 @@
         <v>2018</v>
       </c>
       <c r="C10">
-        <v>285000</v>
+        <v>266400</v>
       </c>
       <c r="D10" s="1">
-        <v>11337</v>
+        <v>1767</v>
       </c>
       <c r="E10">
-        <v>6041.56</v>
+        <v>5391.93</v>
       </c>
       <c r="F10">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="G10" s="1">
-        <v>45100</v>
+        <v>21500</v>
       </c>
       <c r="H10">
-        <v>346836</v>
+        <v>300355</v>
       </c>
       <c r="I10" s="1">
-        <v>2105228</v>
+        <v>612103</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -726,187 +738,187 @@
         <v>2019</v>
       </c>
       <c r="C11">
-        <v>272700</v>
+        <v>277300</v>
       </c>
       <c r="D11" s="1">
-        <v>11277</v>
+        <v>1799</v>
       </c>
       <c r="E11">
-        <v>6686.65</v>
+        <v>6279.33</v>
       </c>
       <c r="F11">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="G11" s="1">
-        <v>47100</v>
+        <v>27500</v>
       </c>
       <c r="H11">
-        <v>349654</v>
+        <v>310472</v>
       </c>
       <c r="I11" s="1">
-        <v>2096208</v>
+        <v>627367</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
         <v>2015</v>
       </c>
       <c r="C12">
-        <v>204200</v>
+        <v>256100</v>
       </c>
       <c r="D12" s="1">
-        <v>1584</v>
+        <v>17797</v>
       </c>
       <c r="E12">
-        <v>4750.04</v>
-      </c>
-      <c r="F12">
-        <v>325</v>
+        <v>5727.24</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1500</v>
       </c>
       <c r="G12" s="1">
-        <v>17500</v>
+        <v>31600</v>
       </c>
       <c r="H12">
-        <v>292544</v>
+        <v>307708</v>
       </c>
       <c r="I12" s="1">
-        <v>578067</v>
+        <v>3749412</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13">
+      <c r="B13" s="2">
         <v>2016</v>
       </c>
       <c r="C13">
-        <v>214700</v>
+        <v>261800</v>
       </c>
       <c r="D13" s="1">
-        <v>1712</v>
+        <v>16613</v>
       </c>
       <c r="E13">
-        <v>5012.62</v>
-      </c>
-      <c r="F13">
-        <v>325</v>
+        <v>5589.79</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1440</v>
       </c>
       <c r="G13" s="1">
-        <v>23200</v>
+        <v>32000</v>
       </c>
       <c r="H13">
-        <v>292419</v>
+        <v>307157</v>
       </c>
       <c r="I13" s="1">
-        <v>585891</v>
+        <v>3767892</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14">
+      <c r="B14" s="2">
         <v>2017</v>
       </c>
       <c r="C14">
-        <v>240400</v>
+        <v>272100</v>
       </c>
       <c r="D14" s="1">
-        <v>1762</v>
+        <v>17126</v>
       </c>
       <c r="E14">
-        <v>4713.37</v>
-      </c>
-      <c r="F14">
-        <v>325</v>
+        <v>5731.87</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1440</v>
       </c>
       <c r="G14" s="1">
-        <v>22300</v>
+        <v>33100</v>
       </c>
       <c r="H14">
-        <v>299369</v>
+        <v>313948</v>
       </c>
       <c r="I14" s="1">
-        <v>598819</v>
+        <v>3797118</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15">
+      <c r="B15" s="2">
         <v>2018</v>
       </c>
       <c r="C15">
-        <v>266400</v>
+        <v>275700</v>
       </c>
       <c r="D15" s="1">
-        <v>1767</v>
+        <v>17709</v>
       </c>
       <c r="E15">
-        <v>5391.93</v>
-      </c>
-      <c r="F15">
-        <v>330</v>
+        <v>5685.69</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1435</v>
       </c>
       <c r="G15" s="1">
-        <v>21500</v>
+        <v>35200</v>
       </c>
       <c r="H15">
-        <v>300355</v>
+        <v>320594</v>
       </c>
       <c r="I15" s="1">
-        <v>612103</v>
+        <v>3830309</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16">
+      <c r="B16" s="2">
         <v>2019</v>
       </c>
       <c r="C16">
-        <v>277300</v>
+        <v>282700</v>
       </c>
       <c r="D16" s="1">
-        <v>1799</v>
+        <v>17027</v>
       </c>
       <c r="E16">
-        <v>6279.33</v>
-      </c>
-      <c r="F16">
-        <v>280</v>
+        <v>5873.28</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1415</v>
       </c>
       <c r="G16" s="1">
-        <v>27500</v>
+        <v>36100</v>
       </c>
       <c r="H16">
-        <v>310472</v>
+        <v>325800</v>
       </c>
       <c r="I16" s="1">
-        <v>627367</v>
+        <v>3876364</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2">
         <v>2015</v>
       </c>
       <c r="C17">
-        <v>256100</v>
+        <v>199800</v>
       </c>
       <c r="D17" s="1">
-        <v>17797</v>
+        <v>17835</v>
       </c>
       <c r="E17">
-        <v>5727.24</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1500</v>
+        <v>5478.74</v>
+      </c>
+      <c r="F17">
+        <v>900</v>
       </c>
       <c r="G17" s="1">
-        <v>31600</v>
+        <v>25400</v>
       </c>
       <c r="H17">
-        <v>307708</v>
+        <v>289735</v>
       </c>
       <c r="I17" s="1">
-        <v>3749412</v>
+        <v>3037185</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -914,25 +926,25 @@
         <v>2016</v>
       </c>
       <c r="C18">
-        <v>261800</v>
+        <v>207800</v>
       </c>
       <c r="D18" s="1">
-        <v>16613</v>
+        <v>18723</v>
       </c>
       <c r="E18">
-        <v>5589.79</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1440</v>
+        <v>5276.22</v>
+      </c>
+      <c r="F18">
+        <v>900</v>
       </c>
       <c r="G18" s="1">
-        <v>32000</v>
+        <v>31300</v>
       </c>
       <c r="H18">
-        <v>307157</v>
+        <v>294947</v>
       </c>
       <c r="I18" s="1">
-        <v>3767892</v>
+        <v>3051063</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -940,25 +952,25 @@
         <v>2017</v>
       </c>
       <c r="C19">
-        <v>272100</v>
+        <v>208200</v>
       </c>
       <c r="D19" s="1">
-        <v>17126</v>
+        <v>17629</v>
       </c>
       <c r="E19">
-        <v>5731.87</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1440</v>
+        <v>5753.3</v>
+      </c>
+      <c r="F19">
+        <v>880</v>
       </c>
       <c r="G19" s="1">
-        <v>33100</v>
+        <v>32500</v>
       </c>
       <c r="H19">
-        <v>313948</v>
+        <v>302207</v>
       </c>
       <c r="I19" s="1">
-        <v>3797118</v>
+        <v>3063986</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -966,25 +978,25 @@
         <v>2018</v>
       </c>
       <c r="C20">
-        <v>275700</v>
+        <v>214800</v>
       </c>
       <c r="D20" s="1">
-        <v>17709</v>
+        <v>17648</v>
       </c>
       <c r="E20">
-        <v>5685.69</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1435</v>
+        <v>6055.68</v>
+      </c>
+      <c r="F20">
+        <v>880</v>
       </c>
       <c r="G20" s="1">
-        <v>35200</v>
+        <v>31800</v>
       </c>
       <c r="H20">
-        <v>320594</v>
+        <v>306908</v>
       </c>
       <c r="I20" s="1">
-        <v>3830309</v>
+        <v>3079425</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -992,54 +1004,54 @@
         <v>2019</v>
       </c>
       <c r="C21">
-        <v>282700</v>
+        <v>218100</v>
       </c>
       <c r="D21" s="1">
-        <v>17027</v>
+        <v>16833</v>
       </c>
       <c r="E21">
-        <v>5873.28</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1415</v>
+        <v>6752.37</v>
+      </c>
+      <c r="F21">
+        <v>900</v>
       </c>
       <c r="G21" s="1">
-        <v>36100</v>
+        <v>31900</v>
       </c>
       <c r="H21">
-        <v>325800</v>
+        <v>313579</v>
       </c>
       <c r="I21" s="1">
-        <v>3876364</v>
+        <v>3104622</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
         <v>2015</v>
       </c>
       <c r="C22">
-        <v>199800</v>
+        <v>305800</v>
       </c>
       <c r="D22" s="1">
-        <v>17835</v>
+        <v>90142</v>
       </c>
       <c r="E22">
-        <v>5478.74</v>
-      </c>
-      <c r="F22">
-        <v>900</v>
+        <v>4252.49</v>
+      </c>
+      <c r="F22" s="1">
+        <v>34705</v>
       </c>
       <c r="G22" s="1">
-        <v>25400</v>
+        <v>28900</v>
       </c>
       <c r="H22">
-        <v>289735</v>
+        <v>289963</v>
       </c>
       <c r="I22" s="1">
-        <v>3037185</v>
+        <v>32691481</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1047,25 +1059,25 @@
         <v>2016</v>
       </c>
       <c r="C23">
-        <v>207800</v>
+        <v>316000</v>
       </c>
       <c r="D23" s="1">
-        <v>18723</v>
+        <v>88569</v>
       </c>
       <c r="E23">
-        <v>5276.22</v>
-      </c>
-      <c r="F23">
-        <v>900</v>
+        <v>4232.93</v>
+      </c>
+      <c r="F23" s="1">
+        <v>34530</v>
       </c>
       <c r="G23" s="1">
-        <v>31300</v>
+        <v>30400</v>
       </c>
       <c r="H23">
-        <v>294947</v>
+        <v>296890</v>
       </c>
       <c r="I23" s="1">
-        <v>3051063</v>
+        <v>32873351</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1073,25 +1085,25 @@
         <v>2017</v>
       </c>
       <c r="C24">
-        <v>208200</v>
+        <v>327900</v>
       </c>
       <c r="D24" s="1">
-        <v>17629</v>
+        <v>90580</v>
       </c>
       <c r="E24">
-        <v>5753.3</v>
-      </c>
-      <c r="F24">
-        <v>880</v>
+        <v>4329.6499999999996</v>
+      </c>
+      <c r="F24" s="1">
+        <v>34440</v>
       </c>
       <c r="G24" s="1">
         <v>32500</v>
       </c>
       <c r="H24">
-        <v>302207</v>
+        <v>304121</v>
       </c>
       <c r="I24" s="1">
-        <v>3063986</v>
+        <v>33168867</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1099,25 +1111,25 @@
         <v>2018</v>
       </c>
       <c r="C25">
-        <v>214800</v>
+        <v>341000</v>
       </c>
       <c r="D25" s="1">
-        <v>17648</v>
+        <v>91805</v>
       </c>
       <c r="E25">
-        <v>6055.68</v>
-      </c>
-      <c r="F25">
-        <v>880</v>
+        <v>4164.8500000000004</v>
+      </c>
+      <c r="F25" s="1">
+        <v>34805</v>
       </c>
       <c r="G25" s="1">
-        <v>31800</v>
+        <v>34500</v>
       </c>
       <c r="H25">
-        <v>306908</v>
+        <v>313097</v>
       </c>
       <c r="I25" s="1">
-        <v>3079425</v>
+        <v>33554595</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1125,54 +1137,54 @@
         <v>2019</v>
       </c>
       <c r="C26">
-        <v>218100</v>
+        <v>359600</v>
       </c>
       <c r="D26" s="1">
-        <v>16833</v>
+        <v>92857</v>
       </c>
       <c r="E26">
-        <v>6752.37</v>
-      </c>
-      <c r="F26">
-        <v>900</v>
+        <v>4065.71</v>
+      </c>
+      <c r="F26" s="1">
+        <v>35240</v>
       </c>
       <c r="G26" s="1">
-        <v>31900</v>
+        <v>36500</v>
       </c>
       <c r="H26">
-        <v>313579</v>
+        <v>323801</v>
       </c>
       <c r="I26" s="1">
-        <v>3104622</v>
+        <v>33960015</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2">
         <v>2015</v>
       </c>
       <c r="C27">
-        <v>305800</v>
+        <v>455000</v>
       </c>
       <c r="D27" s="1">
-        <v>90142</v>
+        <v>168636</v>
       </c>
       <c r="E27">
-        <v>4252.49</v>
+        <v>4021.58</v>
       </c>
       <c r="F27" s="1">
-        <v>34705</v>
+        <v>91440</v>
       </c>
       <c r="G27" s="1">
-        <v>28900</v>
+        <v>29200</v>
       </c>
       <c r="H27">
-        <v>289963</v>
+        <v>362292</v>
       </c>
       <c r="I27" s="1">
-        <v>32691481</v>
+        <v>54792403</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1180,25 +1192,25 @@
         <v>2016</v>
       </c>
       <c r="C28">
-        <v>316000</v>
+        <v>515200</v>
       </c>
       <c r="D28" s="1">
-        <v>88569</v>
+        <v>165764</v>
       </c>
       <c r="E28">
-        <v>4232.93</v>
+        <v>4090.89</v>
       </c>
       <c r="F28" s="1">
-        <v>34530</v>
+        <v>92575</v>
       </c>
       <c r="G28" s="1">
-        <v>30400</v>
+        <v>30500</v>
       </c>
       <c r="H28">
-        <v>296890</v>
+        <v>367032</v>
       </c>
       <c r="I28" s="1">
-        <v>32873351</v>
+        <v>55411999</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1206,25 +1218,25 @@
         <v>2017</v>
       </c>
       <c r="C29">
-        <v>327900</v>
+        <v>600300</v>
       </c>
       <c r="D29" s="1">
-        <v>90580</v>
+        <v>164381</v>
       </c>
       <c r="E29">
-        <v>4329.6499999999996</v>
+        <v>4259.47</v>
       </c>
       <c r="F29" s="1">
-        <v>34440</v>
+        <v>93480</v>
       </c>
       <c r="G29" s="1">
-        <v>32500</v>
+        <v>31900</v>
       </c>
       <c r="H29">
-        <v>304121</v>
+        <v>376356</v>
       </c>
       <c r="I29" s="1">
-        <v>33168867</v>
+        <v>56199095</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1232,25 +1244,25 @@
         <v>2018</v>
       </c>
       <c r="C30">
-        <v>341000</v>
+        <v>606600</v>
       </c>
       <c r="D30" s="1">
-        <v>91805</v>
+        <v>169954</v>
       </c>
       <c r="E30">
-        <v>4164.8500000000004</v>
+        <v>4509.1499999999996</v>
       </c>
       <c r="F30" s="1">
-        <v>34805</v>
+        <v>94990</v>
       </c>
       <c r="G30" s="1">
         <v>34500</v>
       </c>
       <c r="H30">
-        <v>313097</v>
+        <v>385421</v>
       </c>
       <c r="I30" s="1">
-        <v>33554595</v>
+        <v>57124073</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1258,54 +1270,54 @@
         <v>2019</v>
       </c>
       <c r="C31">
-        <v>359600</v>
+        <v>630600</v>
       </c>
       <c r="D31" s="1">
-        <v>92857</v>
+        <v>170001</v>
       </c>
       <c r="E31">
-        <v>4065.71</v>
+        <v>4544.1000000000004</v>
       </c>
       <c r="F31" s="1">
-        <v>35240</v>
+        <v>96210</v>
       </c>
       <c r="G31" s="1">
-        <v>36500</v>
+        <v>35300</v>
       </c>
       <c r="H31">
-        <v>323801</v>
+        <v>397097</v>
       </c>
       <c r="I31" s="1">
-        <v>33960015</v>
+        <v>58077322</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="2">
         <v>2015</v>
       </c>
       <c r="C32">
-        <v>455000</v>
+        <v>283000</v>
       </c>
       <c r="D32" s="1">
-        <v>168636</v>
+        <v>20876</v>
       </c>
       <c r="E32">
-        <v>4021.58</v>
+        <v>8925.91</v>
       </c>
       <c r="F32" s="1">
-        <v>91440</v>
+        <v>9350</v>
       </c>
       <c r="G32" s="1">
-        <v>29200</v>
-      </c>
-      <c r="H32">
-        <v>362292</v>
+        <v>32700</v>
+      </c>
+      <c r="H32" s="2">
+        <v>342048</v>
       </c>
       <c r="I32" s="1">
-        <v>54792403</v>
+        <v>5164103</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1313,25 +1325,25 @@
         <v>2016</v>
       </c>
       <c r="C33">
-        <v>515200</v>
+        <v>288800</v>
       </c>
       <c r="D33" s="1">
-        <v>165764</v>
+        <v>21317</v>
       </c>
       <c r="E33">
-        <v>4090.89</v>
+        <v>9507.82</v>
       </c>
       <c r="F33" s="1">
-        <v>92575</v>
+        <v>9370</v>
       </c>
       <c r="G33" s="1">
-        <v>30500</v>
-      </c>
-      <c r="H33">
-        <v>367032</v>
+        <v>33500</v>
+      </c>
+      <c r="H33" s="2">
+        <v>344942</v>
       </c>
       <c r="I33" s="1">
-        <v>55411999</v>
+        <v>5244283</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1339,25 +1351,25 @@
         <v>2017</v>
       </c>
       <c r="C34">
-        <v>600300</v>
+        <v>297400</v>
       </c>
       <c r="D34" s="1">
-        <v>164381</v>
+        <v>21879</v>
       </c>
       <c r="E34">
-        <v>4259.47</v>
+        <v>9758.09</v>
       </c>
       <c r="F34" s="1">
-        <v>93480</v>
+        <v>9290</v>
       </c>
       <c r="G34" s="1">
-        <v>31900</v>
-      </c>
-      <c r="H34">
-        <v>376356</v>
+        <v>34400</v>
+      </c>
+      <c r="H34" s="2">
+        <v>356258</v>
       </c>
       <c r="I34" s="1">
-        <v>56199095</v>
+        <v>5327896</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1365,25 +1377,25 @@
         <v>2018</v>
       </c>
       <c r="C35">
-        <v>606600</v>
+        <v>300000</v>
       </c>
       <c r="D35" s="1">
-        <v>169954</v>
+        <v>22753</v>
       </c>
       <c r="E35">
-        <v>4509.1499999999996</v>
+        <v>9998.34</v>
       </c>
       <c r="F35" s="1">
-        <v>94990</v>
+        <v>9330</v>
       </c>
       <c r="G35" s="1">
-        <v>34500</v>
-      </c>
-      <c r="H35">
-        <v>385421</v>
+        <v>35000</v>
+      </c>
+      <c r="H35" s="2">
+        <v>358968</v>
       </c>
       <c r="I35" s="1">
-        <v>57124073</v>
+        <v>5402266</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1391,54 +1403,54 @@
         <v>2019</v>
       </c>
       <c r="C36">
-        <v>630600</v>
+        <v>305200</v>
       </c>
       <c r="D36" s="1">
-        <v>170001</v>
+        <v>22375</v>
       </c>
       <c r="E36">
-        <v>4544.1000000000004</v>
+        <v>10863.72</v>
       </c>
       <c r="F36" s="1">
-        <v>96210</v>
+        <v>9275</v>
       </c>
       <c r="G36" s="1">
-        <v>35300</v>
-      </c>
-      <c r="H36">
-        <v>397097</v>
+        <v>35700</v>
+      </c>
+      <c r="H36" s="2">
+        <v>366168</v>
       </c>
       <c r="I36" s="1">
-        <v>58077322</v>
+        <v>5470522</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" s="2">
         <v>2015</v>
       </c>
       <c r="C37">
-        <v>283000</v>
+        <v>332600</v>
       </c>
       <c r="D37" s="1">
-        <v>20876</v>
-      </c>
-      <c r="E37">
-        <v>8925.91</v>
+        <v>76312</v>
+      </c>
+      <c r="E37" s="3">
+        <v>12919.2</v>
       </c>
       <c r="F37" s="1">
-        <v>9350</v>
+        <v>5605</v>
       </c>
       <c r="G37" s="1">
-        <v>32700</v>
-      </c>
-      <c r="H37" s="2">
-        <v>342048</v>
+        <v>39500</v>
+      </c>
+      <c r="H37">
+        <v>376933</v>
       </c>
       <c r="I37" s="1">
-        <v>5164103</v>
+        <v>4482873</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -1446,25 +1458,25 @@
         <v>2016</v>
       </c>
       <c r="C38">
-        <v>288800</v>
+        <v>332700</v>
       </c>
       <c r="D38" s="1">
-        <v>21317</v>
-      </c>
-      <c r="E38">
-        <v>9507.82</v>
+        <v>72437</v>
+      </c>
+      <c r="E38" s="3">
+        <v>13510.63</v>
       </c>
       <c r="F38" s="1">
-        <v>9370</v>
+        <v>5615</v>
       </c>
       <c r="G38" s="1">
-        <v>33500</v>
-      </c>
-      <c r="H38" s="2">
-        <v>344942</v>
+        <v>38800</v>
+      </c>
+      <c r="H38">
+        <v>371777</v>
       </c>
       <c r="I38" s="1">
-        <v>5244283</v>
+        <v>4535597</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -1472,25 +1484,25 @@
         <v>2017</v>
       </c>
       <c r="C39">
-        <v>297400</v>
+        <v>329900</v>
       </c>
       <c r="D39" s="1">
-        <v>21879</v>
-      </c>
-      <c r="E39">
-        <v>9758.09</v>
+        <v>75669</v>
+      </c>
+      <c r="E39" s="3">
+        <v>12983.31</v>
       </c>
       <c r="F39" s="1">
-        <v>9290</v>
+        <v>5555</v>
       </c>
       <c r="G39" s="1">
-        <v>34400</v>
-      </c>
-      <c r="H39" s="2">
-        <v>356258</v>
+        <v>39900</v>
+      </c>
+      <c r="H39">
+        <v>377344</v>
       </c>
       <c r="I39" s="1">
-        <v>5327896</v>
+        <v>4594617</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -1498,25 +1510,25 @@
         <v>2018</v>
       </c>
       <c r="C40">
-        <v>300000</v>
+        <v>326400</v>
       </c>
       <c r="D40" s="1">
-        <v>22753</v>
-      </c>
-      <c r="E40">
-        <v>9998.34</v>
+        <v>75911</v>
+      </c>
+      <c r="E40" s="3">
+        <v>12665.28</v>
       </c>
       <c r="F40" s="1">
-        <v>9330</v>
+        <v>5490</v>
       </c>
       <c r="G40" s="1">
-        <v>35000</v>
-      </c>
-      <c r="H40" s="2">
-        <v>358968</v>
+        <v>40700</v>
+      </c>
+      <c r="H40">
+        <v>377657</v>
       </c>
       <c r="I40" s="1">
-        <v>5402266</v>
+        <v>4642806</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1524,54 +1536,54 @@
         <v>2019</v>
       </c>
       <c r="C41">
-        <v>305200</v>
+        <v>321700</v>
       </c>
       <c r="D41" s="1">
-        <v>22375</v>
-      </c>
-      <c r="E41">
-        <v>10863.72</v>
+        <v>73865</v>
+      </c>
+      <c r="E41" s="3">
+        <v>12897.62</v>
       </c>
       <c r="F41" s="1">
-        <v>9275</v>
+        <v>5530</v>
       </c>
       <c r="G41" s="1">
-        <v>35700</v>
-      </c>
-      <c r="H41" s="2">
-        <v>366168</v>
+        <v>41300</v>
+      </c>
+      <c r="H41">
+        <v>382286</v>
       </c>
       <c r="I41" s="1">
-        <v>5470522</v>
+        <v>4686750</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B42" s="2">
         <v>2015</v>
       </c>
       <c r="C42">
-        <v>332600</v>
+        <v>432800</v>
       </c>
       <c r="D42" s="1">
-        <v>76312</v>
-      </c>
-      <c r="E42" s="3">
-        <v>12919.2</v>
+        <v>278925</v>
+      </c>
+      <c r="E42" s="2">
+        <v>8916.56</v>
       </c>
       <c r="F42" s="1">
-        <v>5605</v>
+        <v>28465</v>
       </c>
       <c r="G42" s="1">
-        <v>39500</v>
+        <v>41100</v>
       </c>
       <c r="H42">
-        <v>376933</v>
+        <v>457156</v>
       </c>
       <c r="I42" s="1">
-        <v>4482873</v>
+        <v>16548357</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1579,25 +1591,25 @@
         <v>2016</v>
       </c>
       <c r="C43">
-        <v>332700</v>
+        <v>425900</v>
       </c>
       <c r="D43" s="1">
-        <v>72437</v>
-      </c>
-      <c r="E43" s="3">
-        <v>13510.63</v>
+        <v>261747</v>
+      </c>
+      <c r="E43" s="2">
+        <v>9025.9699999999993</v>
       </c>
       <c r="F43" s="1">
-        <v>5615</v>
+        <v>28360</v>
       </c>
       <c r="G43" s="1">
-        <v>38800</v>
+        <v>40600</v>
       </c>
       <c r="H43">
-        <v>371777</v>
+        <v>436067</v>
       </c>
       <c r="I43" s="1">
-        <v>4535597</v>
+        <v>16756614</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -1605,25 +1617,25 @@
         <v>2017</v>
       </c>
       <c r="C44">
-        <v>329900</v>
+        <v>429800</v>
       </c>
       <c r="D44" s="1">
-        <v>75669</v>
-      </c>
-      <c r="E44" s="3">
-        <v>12983.31</v>
+        <v>271617</v>
+      </c>
+      <c r="E44" s="2">
+        <v>9335.17</v>
       </c>
       <c r="F44" s="1">
-        <v>5555</v>
+        <v>28320</v>
       </c>
       <c r="G44" s="1">
-        <v>39900</v>
+        <v>41100</v>
       </c>
       <c r="H44">
-        <v>377344</v>
+        <v>443475</v>
       </c>
       <c r="I44" s="1">
-        <v>4594617</v>
+        <v>16945119</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1631,25 +1643,25 @@
         <v>2018</v>
       </c>
       <c r="C45">
-        <v>326400</v>
+        <v>428500</v>
       </c>
       <c r="D45" s="1">
-        <v>75911</v>
-      </c>
-      <c r="E45" s="3">
-        <v>12665.28</v>
+        <v>276347</v>
+      </c>
+      <c r="E45" s="2">
+        <v>9392.19</v>
       </c>
       <c r="F45" s="1">
-        <v>5490</v>
+        <v>28565</v>
       </c>
       <c r="G45" s="1">
-        <v>40700</v>
+        <v>42400</v>
       </c>
       <c r="H45">
-        <v>377657</v>
+        <v>447687</v>
       </c>
       <c r="I45" s="1">
-        <v>4642806</v>
+        <v>17166499</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1657,54 +1669,54 @@
         <v>2019</v>
       </c>
       <c r="C46">
-        <v>321700</v>
+        <v>420900</v>
       </c>
       <c r="D46" s="1">
-        <v>73865</v>
-      </c>
-      <c r="E46" s="3">
-        <v>12897.62</v>
+        <v>278980</v>
+      </c>
+      <c r="E46" s="2">
+        <v>10026.65</v>
       </c>
       <c r="F46" s="1">
-        <v>5530</v>
+        <v>29015</v>
       </c>
       <c r="G46" s="1">
-        <v>41300</v>
+        <v>43100</v>
       </c>
       <c r="H46">
-        <v>382286</v>
+        <v>455768</v>
       </c>
       <c r="I46" s="1">
-        <v>4686750</v>
+        <v>17422845</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B47" s="2">
         <v>2015</v>
       </c>
       <c r="C47">
-        <v>432800</v>
+        <v>610000</v>
       </c>
       <c r="D47" s="1">
-        <v>278925</v>
-      </c>
-      <c r="E47" s="2">
-        <v>8916.56</v>
+        <v>80171</v>
+      </c>
+      <c r="E47">
+        <v>8608.09</v>
       </c>
       <c r="F47" s="1">
-        <v>28465</v>
+        <v>33105</v>
       </c>
       <c r="G47" s="1">
-        <v>41100</v>
+        <v>28800</v>
       </c>
       <c r="H47">
-        <v>457156</v>
+        <v>346298</v>
       </c>
       <c r="I47" s="1">
-        <v>16548357</v>
+        <v>19082570</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1712,235 +1724,102 @@
         <v>2016</v>
       </c>
       <c r="C48">
-        <v>425900</v>
+        <v>717600</v>
       </c>
       <c r="D48" s="1">
-        <v>261747</v>
-      </c>
-      <c r="E48" s="2">
-        <v>9025.9699999999993</v>
+        <v>80291</v>
+      </c>
+      <c r="E48">
+        <v>8488.51</v>
       </c>
       <c r="F48" s="1">
-        <v>28360</v>
+        <v>33290</v>
       </c>
       <c r="G48" s="1">
-        <v>40600</v>
+        <v>30700</v>
       </c>
       <c r="H48">
-        <v>436067</v>
+        <v>351579</v>
       </c>
       <c r="I48" s="1">
-        <v>16756614</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19386872</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="2">
         <v>2017</v>
       </c>
       <c r="C49">
-        <v>429800</v>
+        <v>775400</v>
       </c>
       <c r="D49" s="1">
-        <v>271617</v>
-      </c>
-      <c r="E49" s="2">
-        <v>9335.17</v>
+        <v>81521</v>
+      </c>
+      <c r="E49">
+        <v>8090.02</v>
       </c>
       <c r="F49" s="1">
-        <v>28320</v>
+        <v>33495</v>
       </c>
       <c r="G49" s="1">
-        <v>41100</v>
+        <v>32500</v>
       </c>
       <c r="H49">
-        <v>443475</v>
+        <v>362511</v>
       </c>
       <c r="I49" s="1">
-        <v>16945119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19681992</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
         <v>2018</v>
       </c>
       <c r="C50">
-        <v>428500</v>
+        <v>816300</v>
       </c>
       <c r="D50" s="1">
-        <v>276347</v>
-      </c>
-      <c r="E50" s="2">
-        <v>9392.19</v>
+        <v>83054</v>
+      </c>
+      <c r="E50">
+        <v>8250.9500000000007</v>
       </c>
       <c r="F50" s="1">
-        <v>28565</v>
+        <v>33725</v>
       </c>
       <c r="G50" s="1">
-        <v>42400</v>
+        <v>34400</v>
       </c>
       <c r="H50">
-        <v>447687</v>
+        <v>368048</v>
       </c>
       <c r="I50" s="1">
-        <v>17166499</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>20001433</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
         <v>2019</v>
       </c>
       <c r="C51">
-        <v>420900</v>
+        <v>785500</v>
       </c>
       <c r="D51" s="1">
-        <v>278980</v>
-      </c>
-      <c r="E51" s="2">
-        <v>10026.65</v>
+        <v>83628</v>
+      </c>
+      <c r="E51">
+        <v>9573.92</v>
       </c>
       <c r="F51" s="1">
-        <v>29015</v>
+        <v>33975</v>
       </c>
       <c r="G51" s="1">
-        <v>43100</v>
+        <v>36400</v>
       </c>
       <c r="H51">
-        <v>455768</v>
+        <v>384468</v>
       </c>
       <c r="I51" s="1">
-        <v>17422845</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="2">
-        <v>2015</v>
-      </c>
-      <c r="C52">
-        <v>610000</v>
-      </c>
-      <c r="D52" s="1">
-        <v>80171</v>
-      </c>
-      <c r="E52">
-        <v>8608.09</v>
-      </c>
-      <c r="F52" s="1">
-        <v>33105</v>
-      </c>
-      <c r="G52" s="1">
-        <v>28800</v>
-      </c>
-      <c r="H52">
-        <v>346298</v>
-      </c>
-      <c r="I52" s="1">
-        <v>19082570</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B53" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C53">
-        <v>717600</v>
-      </c>
-      <c r="D53" s="1">
-        <v>80291</v>
-      </c>
-      <c r="E53">
-        <v>8488.51</v>
-      </c>
-      <c r="F53" s="1">
-        <v>33290</v>
-      </c>
-      <c r="G53" s="1">
-        <v>30700</v>
-      </c>
-      <c r="H53">
-        <v>351579</v>
-      </c>
-      <c r="I53" s="1">
-        <v>19386872</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="2">
-        <v>2017</v>
-      </c>
-      <c r="C54">
-        <v>775400</v>
-      </c>
-      <c r="D54" s="1">
-        <v>81521</v>
-      </c>
-      <c r="E54">
-        <v>8090.02</v>
-      </c>
-      <c r="F54" s="1">
-        <v>33495</v>
-      </c>
-      <c r="G54" s="1">
-        <v>32500</v>
-      </c>
-      <c r="H54">
-        <v>362511</v>
-      </c>
-      <c r="I54" s="1">
-        <v>19681992</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B55" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C55">
-        <v>816300</v>
-      </c>
-      <c r="D55" s="1">
-        <v>83054</v>
-      </c>
-      <c r="E55">
-        <v>8250.9500000000007</v>
-      </c>
-      <c r="F55" s="1">
-        <v>33725</v>
-      </c>
-      <c r="G55" s="1">
-        <v>34400</v>
-      </c>
-      <c r="H55">
-        <v>368048</v>
-      </c>
-      <c r="I55" s="1">
-        <v>20001433</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B56" s="2">
-        <v>2019</v>
-      </c>
-      <c r="C56">
-        <v>785500</v>
-      </c>
-      <c r="D56" s="1">
-        <v>83628</v>
-      </c>
-      <c r="E56">
-        <v>9573.92</v>
-      </c>
-      <c r="F56" s="1">
-        <v>33975</v>
-      </c>
-      <c r="G56" s="1">
-        <v>36400</v>
-      </c>
-      <c r="H56">
-        <v>384468</v>
-      </c>
-      <c r="I56" s="1">
         <v>20339311</v>
       </c>
     </row>

</xml_diff>